<commit_message>
Export to .xlsx files, Heroku deployment
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/files/expenses.xlsx
+++ b/src/main/webapp/resources/files/expenses.xlsx
@@ -5,107 +5,178 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Pablo/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Pablo/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5083259C-EC45-6346-B490-44FDF8C9AC69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3A212F-7A83-8C4B-BB6E-B180470CC5B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{7A82187A-6FC1-F94E-90C6-DC00D761843A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Audi A4 B6 1.8T" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type </t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>milage</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>litres</t>
-  </si>
-  <si>
-    <t>level</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>Serwis hamulców</t>
-  </si>
-  <si>
-    <t>150.49</t>
-  </si>
-  <si>
-    <t>Klocki TRW</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Milage</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Litres</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Badanie techniczne</t>
+  </si>
+  <si>
+    <t>MOT</t>
+  </si>
+  <si>
+    <t>2020-02-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Pierwsze badanie techniczne w kraju.</t>
+  </si>
+  <si>
+    <t>Polisa OC</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>2020-02-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTU OC+NNW </t>
+  </si>
+  <si>
+    <t>Pompka spryskiwacza</t>
+  </si>
+  <si>
+    <t>Repairs</t>
+  </si>
+  <si>
+    <t>2020-03-02</t>
+  </si>
+  <si>
+    <t>Pompka spryskiwacza reflektorów</t>
+  </si>
+  <si>
+    <t>Żarówki</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Żarówki świateł mijania Bosch Xenon Blue H7</t>
+  </si>
+  <si>
+    <t>Rozrząd, olej, filtry</t>
+  </si>
+  <si>
+    <t>Exploitation</t>
+  </si>
+  <si>
+    <t>2020-03-05</t>
+  </si>
+  <si>
+    <t>Zestaw rozrządu, pompa wody, pasek wielorowkowy, rolka napinacza paska, rolka prowadząca pasek, olej Castrol 5W30, filtr oleju, filtr kabinowy, płyn chłodniczy, zawór DV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Świece </t>
+  </si>
+  <si>
+    <t>2020-03-06</t>
+  </si>
+  <si>
+    <t>Świece NGK PRF6Q</t>
+  </si>
+  <si>
+    <t>Wycieraczki</t>
+  </si>
+  <si>
+    <t>2020-03-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wymiana wycieraczek </t>
+  </si>
+  <si>
+    <t>Intercooler BEX</t>
+  </si>
+  <si>
+    <t>2020-04-06</t>
+  </si>
+  <si>
+    <t>Montaż drugiego intercoolera</t>
+  </si>
+  <si>
+    <t>Czujnik ECT</t>
+  </si>
+  <si>
+    <t>2020-04-09</t>
+  </si>
+  <si>
+    <t>Wymiana czujnika temperatury cieczy chłodzącej</t>
+  </si>
+  <si>
+    <t>Katalizator sportowy</t>
+  </si>
+  <si>
+    <t>2020-04-28</t>
+  </si>
+  <si>
+    <t>Katalizator sportowy + montaż + złącze elastyczne + naprawa wydechu</t>
   </si>
   <si>
     <t>PB</t>
   </si>
   <si>
-    <t>211.12</t>
-  </si>
-  <si>
-    <t>LPG</t>
-  </si>
-  <si>
-    <t>100.11</t>
-  </si>
-  <si>
-    <t>Wymiana oleju</t>
-  </si>
-  <si>
-    <t>149.00</t>
-  </si>
-  <si>
-    <t>Olej 5W40</t>
+    <t>Fuel</t>
+  </si>
+  <si>
+    <t>2020-02-15</t>
+  </si>
+  <si>
+    <t>2020-02-26</t>
+  </si>
+  <si>
+    <t>2020-02-27</t>
+  </si>
+  <si>
+    <t>2020-04-10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,11 +202,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -449,42 +518,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75C2719-125C-B748-A556-C02F2DFAF343}">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -492,86 +560,390 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>43955</v>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>211000</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
+        <v>105729</v>
+      </c>
+      <c r="E2">
+        <v>99.989997863769531</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2">
-        <v>43924</v>
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="D3">
-        <v>210530</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3">
-        <v>50</v>
-      </c>
-      <c r="G3">
-        <v>60</v>
+        <v>105729</v>
+      </c>
+      <c r="E3">
+        <v>706</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2">
-        <v>43924</v>
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D4">
-        <v>210530</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4">
-        <v>49</v>
-      </c>
-      <c r="G4">
-        <v>49</v>
+        <v>106000</v>
+      </c>
+      <c r="E4">
+        <v>69.529998779296875</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
-        <v>43892</v>
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D5">
-        <v>209454</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
+        <v>106000</v>
+      </c>
+      <c r="E5">
+        <v>91.699996948242188</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>106190</v>
+      </c>
+      <c r="E6">
+        <v>1400</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7">
+        <v>106250</v>
+      </c>
+      <c r="E7">
+        <v>179.96000671386719</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8">
+        <v>106404</v>
+      </c>
+      <c r="E8">
+        <v>44.799999237060547</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9">
+        <v>106660</v>
+      </c>
+      <c r="E9">
+        <v>650</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10">
+        <v>106660</v>
+      </c>
+      <c r="E10">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11">
+        <v>106900</v>
+      </c>
+      <c r="E11">
+        <v>1175</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12">
+        <v>105638</v>
+      </c>
+      <c r="E12">
+        <v>141.41999816894531</v>
+      </c>
+      <c r="F12">
+        <v>30.090000152587891</v>
+      </c>
+      <c r="G12">
+        <v>33</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13">
+        <v>105863</v>
+      </c>
+      <c r="E13">
+        <v>100.76999664306641</v>
+      </c>
+      <c r="F13">
+        <v>21.350000381469727</v>
+      </c>
+      <c r="G13">
+        <v>33</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14">
+        <v>105987</v>
+      </c>
+      <c r="E14">
+        <v>150.25999450683594</v>
+      </c>
+      <c r="F14">
+        <v>31.239999771118164</v>
+      </c>
+      <c r="G14">
+        <v>57</v>
+      </c>
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15">
+        <v>106404</v>
+      </c>
+      <c r="E15">
+        <v>256.25</v>
+      </c>
+      <c r="F15">
+        <v>54.290000915527344</v>
+      </c>
+      <c r="G15">
+        <v>66</v>
+      </c>
+      <c r="H15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16">
+        <v>106663</v>
+      </c>
+      <c r="E16">
+        <v>112.30999755859375</v>
+      </c>
+      <c r="F16">
+        <v>27.729999542236328</v>
+      </c>
+      <c r="G16">
+        <v>66</v>
+      </c>
+      <c r="H16" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>